<commit_message>
fixed due date format
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -40,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -53,6 +53,27 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -429,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +478,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>fda</t>
+          <t>fdad</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
@@ -465,19 +486,41 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>44594</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>1</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
       </c>
-      <c r="E2" s="2" t="n">
+      <c r="E3" s="2" t="n">
         <v>40544</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed a item name bug
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -16,14 +16,20 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD"/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +48,22 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,14 +429,78 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>priority</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>due_date</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>daf</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>dwq</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>44655</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>fda</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>44988</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
seperated class from main.py, added comments, fixed typo
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +457,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>daf</t>
+          <t>dafd</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
@@ -465,7 +465,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>dwq</t>
+          <t>d</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -474,30 +474,7 @@
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>44655</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>fda</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>44988</v>
+        <v>44594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed obtain item name bug
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -40,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -53,6 +53,27 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -429,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +478,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>dafd</t>
+          <t>fda</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
@@ -465,7 +486,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>fda</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -477,7 +498,29 @@
         <v>44594</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>daf</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>44594</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed obtain list name func
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -40,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -53,27 +53,6 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -450,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +457,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>fda</t>
+          <t>fdafd</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
@@ -486,41 +465,19 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>fda</t>
+          <t>fd</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
         <v>44594</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="1" t="n"/>
-      <c r="B3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>daf</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>44594</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A2:A3"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changed quit selection for remove item
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -40,7 +40,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -53,6 +53,27 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
@@ -429,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +478,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>fds</t>
+          <t>test</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
@@ -465,19 +486,60 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>fda</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>3</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>48641</v>
+        <v>40544</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>40524</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>added</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>44594</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A4"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add shell script file
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -450,7 +450,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +478,7 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>export</t>
         </is>
       </c>
       <c r="B2" s="1" t="n">
@@ -486,16 +486,16 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>test</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>1</t>
+          <t>2</t>
         </is>
       </c>
       <c r="E2" s="2" t="n">
-        <v>40544</v>
+        <v>44594</v>
       </c>
     </row>
     <row r="3">
@@ -505,40 +505,21 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>test2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>2</t>
+          <t>1</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>40524</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="1" t="n"/>
-      <c r="B4" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>added</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>44594</v>
+        <v>44844</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:A4"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>